<commit_message>
uploaded example excel file
</commit_message>
<xml_diff>
--- a/example-input-data.xlsx
+++ b/example-input-data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/96ec78218e4788a4/Documents/comp4710/comp-4710-data-mining-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/96ec78218e4788a4/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5D2E3AA-EECB-4ADB-A11D-30FAAFB5A85F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{F3F31224-5F61-4549-86E1-132F0E16EFEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2930" yWindow="0" windowWidth="16180" windowHeight="8560" xr2:uid="{E87DD0B6-E7B2-4157-B8AC-805C31E86C86}"/>
   </bookViews>
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82392CB-FBB5-4DA2-998E-96130B706B33}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="96" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="96" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>